<commit_message>
Added all Teaching and learning tools
</commit_message>
<xml_diff>
--- a/KS1/Year-2.xlsx
+++ b/KS1/Year-2.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="102">
   <si>
     <t>Lesson</t>
   </si>
@@ -204,9 +204,6 @@
     <t>I can use their algorithm To create a program                                              I can test and debug each part of the program</t>
   </si>
   <si>
-    <t>Data Science (DS)</t>
-  </si>
-  <si>
     <t>Pictograms</t>
   </si>
   <si>
@@ -369,20 +366,69 @@
 - I can use more than one block by joining them together</t>
   </si>
   <si>
-    <t>KS1</t>
-  </si>
-  <si>
     <t>Computing Concepts (CC)</t>
   </si>
   <si>
     <t>Five-Eight</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Desktop or Laptop (Hardware)                                                                                       paint tool or</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="4" tint="-0.499984740745262"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">paintz.app  (Software)      </t>
+    </r>
+  </si>
+  <si>
+    <t>Digital Camera</t>
+  </si>
+  <si>
+    <t>Bee-Bot                                                                                                                                         Blue-Bot,                                                                                                        or other fixed-movement floor robot</t>
+  </si>
+  <si>
+    <t>Computing Concepts (CC</t>
+  </si>
+  <si>
+    <t>https://www.j2e.com/jit5#pictogram</t>
+  </si>
+  <si>
+    <t>https://musiclab.chromeexperiments.com/</t>
+  </si>
+  <si>
+    <t>ScratchJr (Tablet)                                                                                                     Scratch Offline Editor (Desktop/Laptop)                                                                            scratch.mit.edu (Web)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="9">
+  <fonts count="13">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -442,8 +488,39 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color theme="4" tint="-0.499984740745262"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -470,12 +547,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="2" tint="-0.14999847407452621"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -496,6 +567,24 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor theme="0"/>
       </patternFill>
     </fill>
   </fills>
@@ -641,20 +730,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -740,12 +827,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -764,91 +845,84 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="36">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFCCCCCC"/>
-          <bgColor rgb="FFCCCCCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFEFEFEF"/>
-          <bgColor rgb="FFEFEFEF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFCCCCCC"/>
-          <bgColor rgb="FFCCCCCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFEFEFEF"/>
-          <bgColor rgb="FFEFEFEF"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="32">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -1313,1037 +1387,1085 @@
   </sheetPr>
   <dimension ref="A1:M26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="12.7109375" style="33"/>
+    <col min="1" max="1" width="12.7109375" style="31"/>
     <col min="2" max="2" width="9" customWidth="1"/>
     <col min="3" max="3" width="12.140625" customWidth="1"/>
-    <col min="4" max="4" width="23.42578125" style="29" customWidth="1"/>
-    <col min="5" max="5" width="24.28515625" style="42" customWidth="1"/>
+    <col min="4" max="4" width="23.42578125" style="27" customWidth="1"/>
+    <col min="5" max="5" width="24.28515625" style="38" customWidth="1"/>
     <col min="6" max="6" width="11.7109375" customWidth="1"/>
-    <col min="7" max="7" width="11" style="29" customWidth="1"/>
-    <col min="8" max="8" width="9.85546875" style="29" customWidth="1"/>
+    <col min="7" max="7" width="11" style="27" customWidth="1"/>
+    <col min="8" max="8" width="9.85546875" style="27" customWidth="1"/>
     <col min="9" max="9" width="39.7109375" customWidth="1"/>
-    <col min="10" max="10" width="16.140625" style="29" customWidth="1"/>
-    <col min="11" max="11" width="58.85546875" style="29" customWidth="1"/>
+    <col min="10" max="10" width="51.85546875" style="27" customWidth="1"/>
+    <col min="11" max="11" width="58.85546875" style="59" customWidth="1"/>
     <col min="12" max="12" width="47.85546875" customWidth="1"/>
     <col min="13" max="13" width="29.7109375" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="12.95" customHeight="1">
+    <row r="1" spans="1:13" ht="12.75" hidden="1" customHeight="1">
       <c r="B1" s="1"/>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
-      <c r="E1" s="37"/>
+      <c r="E1" s="33"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
+      <c r="K1" s="58"/>
       <c r="L1" s="2"/>
       <c r="M1" s="3"/>
     </row>
-    <row r="2" spans="1:13" ht="36.75" customHeight="1" thickBot="1">
-      <c r="A2" s="35" t="s">
+    <row r="2" spans="1:13" s="57" customFormat="1" ht="36.75" customHeight="1" thickBot="1">
+      <c r="A2" s="53" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="54" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="4" t="s">
+      <c r="C2" s="54" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="54" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="54" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="G2" s="54" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="4" t="s">
+      <c r="H2" s="54" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="J2" s="4" t="s">
+      <c r="I2" s="54" t="s">
+        <v>1</v>
+      </c>
+      <c r="J2" s="55" t="s">
         <v>11</v>
       </c>
-      <c r="K2" s="4" t="s">
+      <c r="K2" s="54" t="s">
         <v>12</v>
       </c>
-      <c r="L2" s="4" t="s">
+      <c r="L2" s="54" t="s">
         <v>13</v>
       </c>
-      <c r="M2" s="5"/>
+      <c r="M2" s="56"/>
     </row>
     <row r="3" spans="1:13" ht="64.5" customHeight="1">
-      <c r="A3" s="34" t="s">
+      <c r="A3" s="32">
+        <v>1</v>
+      </c>
+      <c r="B3" s="4">
+        <v>2</v>
+      </c>
+      <c r="C3" s="28" t="s">
         <v>94</v>
       </c>
-      <c r="B3" s="6">
-        <v>2</v>
-      </c>
-      <c r="C3" s="30" t="s">
-        <v>96</v>
-      </c>
-      <c r="D3" s="30" t="s">
+      <c r="D3" s="28" t="s">
+        <v>93</v>
+      </c>
+      <c r="E3" s="34" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="5">
+        <v>1</v>
+      </c>
+      <c r="G3" s="5">
+        <v>1</v>
+      </c>
+      <c r="H3" s="5">
+        <v>1</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="J3" s="51" t="s">
         <v>95</v>
       </c>
-      <c r="E3" s="38" t="s">
+      <c r="K3" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="L3" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="M3" s="8">
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("ArrayFormula(COUNTUNIQUE($C$3:C3))"),1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="66.75" customHeight="1">
+      <c r="A4" s="32">
+        <v>1</v>
+      </c>
+      <c r="B4" s="9">
+        <v>2</v>
+      </c>
+      <c r="C4" s="28" t="s">
+        <v>94</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="E4" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="7">
-        <v>1</v>
-      </c>
-      <c r="G3" s="7">
-        <v>1</v>
-      </c>
-      <c r="H3" s="7">
-        <v>1</v>
-      </c>
-      <c r="I3" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="J3" s="8"/>
-      <c r="K3" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="L3" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="M3" s="10">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("ArrayFormula(COUNTUNIQUE($C$3:C3))"),1)</f>
+      <c r="F4" s="10">
+        <v>2</v>
+      </c>
+      <c r="G4" s="10">
+        <v>1</v>
+      </c>
+      <c r="H4" s="10">
+        <v>2</v>
+      </c>
+      <c r="I4" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="J4" s="51" t="s">
+        <v>95</v>
+      </c>
+      <c r="K4" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="L4" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="M4" s="13">
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("ArrayFormula(mod(COUNTUNIQUE($C$3:C4),2))"),1)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="51">
-      <c r="A4" s="34" t="s">
+    <row r="5" spans="1:13" ht="60.75" customHeight="1">
+      <c r="A5" s="32">
+        <v>1</v>
+      </c>
+      <c r="B5" s="9">
+        <v>2</v>
+      </c>
+      <c r="C5" s="28" t="s">
         <v>94</v>
       </c>
-      <c r="B4" s="11">
-        <v>2</v>
-      </c>
-      <c r="C4" s="30" t="s">
-        <v>96</v>
-      </c>
-      <c r="D4" s="12" t="s">
+      <c r="D5" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="E5" s="35" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" s="10">
+        <v>3</v>
+      </c>
+      <c r="G5" s="10">
+        <v>1</v>
+      </c>
+      <c r="H5" s="10">
+        <v>3</v>
+      </c>
+      <c r="I5" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="J5" s="51" t="s">
         <v>95</v>
       </c>
-      <c r="E4" s="39" t="s">
-        <v>5</v>
-      </c>
-      <c r="F4" s="12">
-        <v>2</v>
-      </c>
-      <c r="G4" s="12">
-        <v>1</v>
-      </c>
-      <c r="H4" s="12">
-        <v>2</v>
-      </c>
-      <c r="I4" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="J4" s="13"/>
-      <c r="K4" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="L4" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="M4" s="15">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("ArrayFormula(mod(COUNTUNIQUE($C$3:C4),2))"),1)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" ht="38.25">
-      <c r="A5" s="34" t="s">
-        <v>94</v>
-      </c>
-      <c r="B5" s="11">
-        <v>2</v>
-      </c>
-      <c r="C5" s="30" t="s">
-        <v>96</v>
-      </c>
-      <c r="D5" s="12" t="s">
-        <v>95</v>
-      </c>
-      <c r="E5" s="39" t="s">
-        <v>5</v>
-      </c>
-      <c r="F5" s="12">
-        <v>3</v>
-      </c>
-      <c r="G5" s="12">
-        <v>1</v>
-      </c>
-      <c r="H5" s="12">
-        <v>3</v>
-      </c>
-      <c r="I5" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="J5" s="13"/>
-      <c r="K5" s="14" t="s">
+      <c r="K5" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="L5" s="14" t="s">
+      <c r="L5" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="M5" s="15">
+      <c r="M5" s="13">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("ArrayFormula(mod(COUNTUNIQUE($C$3:C5),2))"),1)</f>
         <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="62.25" customHeight="1">
-      <c r="A6" s="36" t="s">
+      <c r="A6" s="32">
+        <v>1</v>
+      </c>
+      <c r="B6" s="19">
+        <v>2</v>
+      </c>
+      <c r="C6" s="28" t="s">
         <v>94</v>
       </c>
-      <c r="B6" s="21">
-        <v>2</v>
-      </c>
-      <c r="C6" s="30" t="s">
+      <c r="D6" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="36" t="s">
+        <v>26</v>
+      </c>
+      <c r="F6" s="20">
+        <v>1</v>
+      </c>
+      <c r="G6" s="20">
+        <v>2</v>
+      </c>
+      <c r="H6" s="20">
+        <v>1</v>
+      </c>
+      <c r="I6" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="J6" s="52" t="s">
         <v>96</v>
       </c>
-      <c r="D6" s="22" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" s="40" t="s">
-        <v>26</v>
-      </c>
-      <c r="F6" s="22">
-        <v>1</v>
-      </c>
-      <c r="G6" s="22">
-        <v>2</v>
-      </c>
-      <c r="H6" s="22">
-        <v>1</v>
-      </c>
-      <c r="I6" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="J6" s="23"/>
-      <c r="K6" s="24" t="s">
+      <c r="K6" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="L6" s="24" t="s">
+      <c r="L6" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="M6" s="15">
+      <c r="M6" s="13">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("ArrayFormula(mod(COUNTUNIQUE($C$3:C6),2))"),1)</f>
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="51">
-      <c r="A7" s="36" t="s">
+      <c r="A7" s="32">
+        <v>1</v>
+      </c>
+      <c r="B7" s="9">
+        <v>2</v>
+      </c>
+      <c r="C7" s="28" t="s">
         <v>94</v>
       </c>
-      <c r="B7" s="11">
-        <v>2</v>
-      </c>
-      <c r="C7" s="30" t="s">
+      <c r="D7" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="F7" s="10">
+        <v>2</v>
+      </c>
+      <c r="G7" s="10">
+        <v>2</v>
+      </c>
+      <c r="H7" s="10">
+        <v>2</v>
+      </c>
+      <c r="I7" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="J7" s="52" t="s">
         <v>96</v>
       </c>
-      <c r="D7" s="12" t="s">
+      <c r="K7" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="L7" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="M7" s="13">
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("ArrayFormula(mod(COUNTUNIQUE($C$3:C7),2))"),1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="58.5" customHeight="1">
+      <c r="A8" s="32">
+        <v>1</v>
+      </c>
+      <c r="B8" s="9">
+        <v>2</v>
+      </c>
+      <c r="C8" s="28" t="s">
+        <v>94</v>
+      </c>
+      <c r="D8" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="39" t="s">
+      <c r="E8" s="35" t="s">
         <v>26</v>
       </c>
-      <c r="F7" s="12">
-        <v>2</v>
-      </c>
-      <c r="G7" s="12">
-        <v>2</v>
-      </c>
-      <c r="H7" s="12">
-        <v>2</v>
-      </c>
-      <c r="I7" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="J7" s="13"/>
-      <c r="K7" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="L7" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="M7" s="15">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("ArrayFormula(mod(COUNTUNIQUE($C$3:C7),2))"),1)</f>
+      <c r="F8" s="10">
+        <v>3</v>
+      </c>
+      <c r="G8" s="10">
+        <v>2</v>
+      </c>
+      <c r="H8" s="10">
+        <v>3</v>
+      </c>
+      <c r="I8" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="J8" s="52" t="s">
+        <v>96</v>
+      </c>
+      <c r="K8" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="L8" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="M8" s="18">
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("ArrayFormula(mod(COUNTUNIQUE($C$3:C8),2))"),1)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="49.5" customHeight="1">
-      <c r="A8" s="36" t="s">
+    <row r="9" spans="1:13" ht="87" customHeight="1">
+      <c r="A9" s="32">
+        <v>1</v>
+      </c>
+      <c r="B9" s="19">
+        <v>2</v>
+      </c>
+      <c r="C9" s="28" t="s">
         <v>94</v>
       </c>
-      <c r="B8" s="11">
-        <v>2</v>
-      </c>
-      <c r="C8" s="30" t="s">
-        <v>96</v>
-      </c>
-      <c r="D8" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="E8" s="39" t="s">
-        <v>26</v>
-      </c>
-      <c r="F8" s="12">
+      <c r="D9" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="36" t="s">
+        <v>38</v>
+      </c>
+      <c r="F9" s="20">
+        <v>1</v>
+      </c>
+      <c r="G9" s="20">
         <v>3</v>
       </c>
-      <c r="G8" s="12">
-        <v>2</v>
-      </c>
-      <c r="H8" s="12">
-        <v>3</v>
-      </c>
-      <c r="I8" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="J8" s="13"/>
-      <c r="K8" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="L8" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="M8" s="20">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("ArrayFormula(mod(COUNTUNIQUE($C$3:C8),2))"),1)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" ht="89.25">
-      <c r="A9" s="34" t="s">
-        <v>94</v>
-      </c>
-      <c r="B9" s="21">
-        <v>2</v>
-      </c>
-      <c r="C9" s="30" t="s">
-        <v>96</v>
-      </c>
-      <c r="D9" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="E9" s="40" t="s">
-        <v>38</v>
-      </c>
-      <c r="F9" s="22">
-        <v>1</v>
-      </c>
-      <c r="G9" s="22">
-        <v>3</v>
-      </c>
-      <c r="H9" s="22">
-        <v>1</v>
-      </c>
-      <c r="I9" s="43" t="s">
+      <c r="H9" s="20">
+        <v>1</v>
+      </c>
+      <c r="I9" s="62" t="s">
         <v>40</v>
       </c>
-      <c r="J9" s="23"/>
-      <c r="K9" s="24" t="s">
+      <c r="J9" s="36" t="s">
+        <v>97</v>
+      </c>
+      <c r="K9" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="L9" s="24" t="s">
+      <c r="L9" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="M9" s="25">
+      <c r="M9" s="23">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("ArrayFormula(mod(COUNTUNIQUE($C$3:C9),2))"),0)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="63.75">
-      <c r="A10" s="34" t="s">
+    <row r="10" spans="1:13" ht="72" customHeight="1">
+      <c r="A10" s="32">
+        <v>1</v>
+      </c>
+      <c r="B10" s="9">
+        <v>2</v>
+      </c>
+      <c r="C10" s="28" t="s">
         <v>94</v>
       </c>
-      <c r="B10" s="11">
-        <v>2</v>
-      </c>
-      <c r="C10" s="30" t="s">
-        <v>96</v>
-      </c>
-      <c r="D10" s="12" t="s">
+      <c r="D10" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="E10" s="39" t="s">
+      <c r="E10" s="35" t="s">
         <v>39</v>
       </c>
-      <c r="F10" s="12">
-        <v>2</v>
-      </c>
-      <c r="G10" s="12">
+      <c r="F10" s="10">
+        <v>2</v>
+      </c>
+      <c r="G10" s="10">
         <v>3</v>
       </c>
-      <c r="H10" s="12">
-        <v>2</v>
-      </c>
-      <c r="I10" s="44" t="s">
+      <c r="H10" s="10">
+        <v>2</v>
+      </c>
+      <c r="I10" s="39" t="s">
         <v>41</v>
       </c>
-      <c r="J10" s="13"/>
-      <c r="K10" s="14" t="s">
+      <c r="J10" s="36" t="s">
+        <v>97</v>
+      </c>
+      <c r="K10" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="L10" s="14" t="s">
+      <c r="L10" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="M10" s="26">
+      <c r="M10" s="24">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("ArrayFormula(mod(COUNTUNIQUE($C$3:C10),2))"),0)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="25.5">
-      <c r="A11" s="34" t="s">
+    <row r="11" spans="1:13" ht="72.75" customHeight="1">
+      <c r="A11" s="32">
+        <v>1</v>
+      </c>
+      <c r="B11" s="9">
+        <v>2</v>
+      </c>
+      <c r="C11" s="28" t="s">
         <v>94</v>
       </c>
-      <c r="B11" s="11">
-        <v>2</v>
-      </c>
-      <c r="C11" s="30" t="s">
-        <v>96</v>
-      </c>
-      <c r="D11" s="12" t="s">
+      <c r="D11" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="E11" s="39" t="s">
+      <c r="E11" s="35" t="s">
         <v>38</v>
       </c>
-      <c r="F11" s="12">
+      <c r="F11" s="10">
         <v>3</v>
       </c>
-      <c r="G11" s="12">
+      <c r="G11" s="10">
         <v>3</v>
       </c>
-      <c r="H11" s="12">
+      <c r="H11" s="10">
         <v>3</v>
       </c>
-      <c r="I11" s="44" t="s">
+      <c r="I11" s="39" t="s">
         <v>45</v>
       </c>
-      <c r="J11" s="13"/>
-      <c r="K11" s="14" t="s">
+      <c r="J11" s="36" t="s">
+        <v>97</v>
+      </c>
+      <c r="K11" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="L11" s="14" t="s">
+      <c r="L11" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="M11" s="26">
+      <c r="M11" s="24">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("ArrayFormula(mod(COUNTUNIQUE($C$3:C11),2))"),0)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="38.25">
-      <c r="A12" s="45" t="s">
+    <row r="12" spans="1:13" ht="57" customHeight="1">
+      <c r="A12" s="32">
+        <v>1</v>
+      </c>
+      <c r="B12" s="48">
+        <v>2</v>
+      </c>
+      <c r="C12" s="28" t="s">
         <v>94</v>
       </c>
-      <c r="B12" s="55">
-        <v>2</v>
-      </c>
-      <c r="C12" s="30" t="s">
-        <v>96</v>
-      </c>
-      <c r="D12" s="56" t="s">
+      <c r="D12" s="49" t="s">
+        <v>98</v>
+      </c>
+      <c r="E12" s="41" t="s">
         <v>49</v>
       </c>
-      <c r="E12" s="47" t="s">
-        <v>50</v>
-      </c>
-      <c r="F12" s="46">
-        <v>1</v>
-      </c>
-      <c r="G12" s="46">
+      <c r="F12" s="40">
+        <v>1</v>
+      </c>
+      <c r="G12" s="40">
         <v>4</v>
       </c>
-      <c r="H12" s="46">
-        <v>1</v>
-      </c>
-      <c r="I12" s="48" t="s">
-        <v>52</v>
-      </c>
-      <c r="J12" s="49"/>
-      <c r="K12" s="50" t="s">
-        <v>55</v>
-      </c>
-      <c r="L12" s="50" t="s">
-        <v>57</v>
-      </c>
-      <c r="M12" s="26">
+      <c r="H12" s="40">
+        <v>1</v>
+      </c>
+      <c r="I12" s="42" t="s">
+        <v>51</v>
+      </c>
+      <c r="J12" s="60" t="s">
+        <v>99</v>
+      </c>
+      <c r="K12" s="42" t="s">
+        <v>54</v>
+      </c>
+      <c r="L12" s="44" t="s">
+        <v>56</v>
+      </c>
+      <c r="M12" s="24">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("ArrayFormula(mod(COUNTUNIQUE($C$3:C12),2))"),0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="51">
-      <c r="A13" s="45" t="s">
+      <c r="A13" s="32">
+        <v>1</v>
+      </c>
+      <c r="B13" s="48">
+        <v>2</v>
+      </c>
+      <c r="C13" s="28" t="s">
         <v>94</v>
       </c>
-      <c r="B13" s="55">
-        <v>2</v>
-      </c>
-      <c r="C13" s="30" t="s">
-        <v>96</v>
-      </c>
-      <c r="D13" s="56" t="s">
+      <c r="D13" s="49" t="s">
+        <v>98</v>
+      </c>
+      <c r="E13" s="45" t="s">
         <v>49</v>
       </c>
-      <c r="E13" s="51" t="s">
-        <v>50</v>
-      </c>
-      <c r="F13" s="46">
-        <v>2</v>
-      </c>
-      <c r="G13" s="46">
+      <c r="F13" s="40">
+        <v>2</v>
+      </c>
+      <c r="G13" s="40">
         <v>4</v>
       </c>
-      <c r="H13" s="46">
-        <v>2</v>
-      </c>
-      <c r="I13" s="49" t="s">
-        <v>53</v>
-      </c>
-      <c r="J13" s="49"/>
-      <c r="K13" s="52" t="s">
+      <c r="H13" s="40">
+        <v>2</v>
+      </c>
+      <c r="I13" s="43" t="s">
+        <v>52</v>
+      </c>
+      <c r="J13" s="60" t="s">
+        <v>99</v>
+      </c>
+      <c r="K13" s="43" t="s">
+        <v>57</v>
+      </c>
+      <c r="L13" s="46" t="s">
         <v>58</v>
       </c>
-      <c r="L13" s="52" t="s">
-        <v>59</v>
-      </c>
-      <c r="M13" s="26">
+      <c r="M13" s="24">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("ArrayFormula(mod(COUNTUNIQUE($C$3:C13),2))"),0)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="51">
-      <c r="A14" s="45" t="s">
+    <row r="14" spans="1:13" ht="66" customHeight="1">
+      <c r="A14" s="32">
+        <v>1</v>
+      </c>
+      <c r="B14" s="50">
+        <v>2</v>
+      </c>
+      <c r="C14" s="28" t="s">
         <v>94</v>
       </c>
-      <c r="B14" s="57">
-        <v>2</v>
-      </c>
-      <c r="C14" s="30" t="s">
-        <v>96</v>
-      </c>
-      <c r="D14" s="58" t="s">
-        <v>49</v>
-      </c>
-      <c r="E14" s="51" t="s">
-        <v>51</v>
-      </c>
-      <c r="F14" s="53">
+      <c r="D14" s="49" t="s">
+        <v>98</v>
+      </c>
+      <c r="E14" s="45" t="s">
+        <v>50</v>
+      </c>
+      <c r="F14" s="47">
         <v>3</v>
       </c>
-      <c r="G14" s="53">
+      <c r="G14" s="47">
         <v>4</v>
       </c>
-      <c r="H14" s="53">
+      <c r="H14" s="47">
         <v>3</v>
       </c>
-      <c r="I14" s="49" t="s">
-        <v>54</v>
-      </c>
-      <c r="J14" s="54"/>
-      <c r="K14" s="52" t="s">
-        <v>56</v>
-      </c>
-      <c r="L14" s="52" t="s">
-        <v>56</v>
-      </c>
-      <c r="M14" s="27">
+      <c r="I14" s="43" t="s">
+        <v>53</v>
+      </c>
+      <c r="J14" s="60" t="s">
+        <v>99</v>
+      </c>
+      <c r="K14" s="43" t="s">
+        <v>55</v>
+      </c>
+      <c r="L14" s="46" t="s">
+        <v>55</v>
+      </c>
+      <c r="M14" s="25">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("ArrayFormula(mod(COUNTUNIQUE($C$3:C14),2))"),0)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="38.25">
-      <c r="A15" s="34" t="s">
+    <row r="15" spans="1:13" ht="68.25" customHeight="1">
+      <c r="A15" s="32">
+        <v>1</v>
+      </c>
+      <c r="B15" s="9">
+        <v>2</v>
+      </c>
+      <c r="C15" s="28" t="s">
         <v>94</v>
       </c>
-      <c r="B15" s="11">
-        <v>2</v>
-      </c>
-      <c r="C15" s="30" t="s">
-        <v>96</v>
-      </c>
-      <c r="D15" s="12" t="s">
+      <c r="D15" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="E15" s="39" t="s">
+      <c r="E15" s="35" t="s">
+        <v>59</v>
+      </c>
+      <c r="F15" s="10">
+        <v>1</v>
+      </c>
+      <c r="G15" s="10">
+        <v>5</v>
+      </c>
+      <c r="H15" s="10">
+        <v>1</v>
+      </c>
+      <c r="I15" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="F15" s="12">
-        <v>1</v>
-      </c>
-      <c r="G15" s="12">
+      <c r="J15" s="61" t="s">
+        <v>100</v>
+      </c>
+      <c r="K15" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="L15" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="M15" s="26">
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("ArrayFormula(mod(COUNTUNIQUE($C$3:C15),2))"),1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="68.25" customHeight="1">
+      <c r="A16" s="32">
+        <v>1</v>
+      </c>
+      <c r="B16" s="9">
+        <v>2</v>
+      </c>
+      <c r="C16" s="28" t="s">
+        <v>94</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E16" s="35" t="s">
+        <v>59</v>
+      </c>
+      <c r="F16" s="10">
+        <v>2</v>
+      </c>
+      <c r="G16" s="10">
         <v>5</v>
       </c>
-      <c r="H15" s="12">
-        <v>1</v>
-      </c>
-      <c r="I15" s="13" t="s">
+      <c r="H16" s="10">
+        <v>2</v>
+      </c>
+      <c r="I16" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="J15" s="13"/>
-      <c r="K15" s="14" t="s">
+      <c r="J16" s="61" t="s">
+        <v>100</v>
+      </c>
+      <c r="K16" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="L16" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="M16" s="13">
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("ArrayFormula(mod(COUNTUNIQUE($C$3:C16),2))"),1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" ht="68.25" customHeight="1">
+      <c r="A17" s="32">
+        <v>1</v>
+      </c>
+      <c r="B17" s="14">
+        <v>2</v>
+      </c>
+      <c r="C17" s="28" t="s">
+        <v>94</v>
+      </c>
+      <c r="D17" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E17" s="37" t="s">
+        <v>59</v>
+      </c>
+      <c r="F17" s="15">
+        <v>3</v>
+      </c>
+      <c r="G17" s="15">
+        <v>5</v>
+      </c>
+      <c r="H17" s="15">
+        <v>3</v>
+      </c>
+      <c r="I17" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="J17" s="61" t="s">
+        <v>100</v>
+      </c>
+      <c r="K17" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="L17" s="17" t="s">
+        <v>67</v>
+      </c>
+      <c r="M17" s="13">
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("ArrayFormula(mod(COUNTUNIQUE($C$3:C17),2))"),1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" ht="65.25" customHeight="1">
+      <c r="A18" s="32">
+        <v>1</v>
+      </c>
+      <c r="B18" s="9">
+        <v>2</v>
+      </c>
+      <c r="C18" s="28" t="s">
+        <v>94</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E18" s="35" t="s">
+        <v>59</v>
+      </c>
+      <c r="F18" s="10">
+        <v>1</v>
+      </c>
+      <c r="G18" s="10">
+        <v>6</v>
+      </c>
+      <c r="H18" s="10">
+        <v>1</v>
+      </c>
+      <c r="I18" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="J18" s="61" t="s">
+        <v>100</v>
+      </c>
+      <c r="K18" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="L18" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="M18" s="13">
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("ArrayFormula(mod(COUNTUNIQUE($C$3:C18),2))"),1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" ht="65.25" customHeight="1">
+      <c r="A19" s="32">
+        <v>1</v>
+      </c>
+      <c r="B19" s="9">
+        <v>2</v>
+      </c>
+      <c r="C19" s="28" t="s">
+        <v>94</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E19" s="35" t="s">
+        <v>59</v>
+      </c>
+      <c r="F19" s="10">
+        <v>2</v>
+      </c>
+      <c r="G19" s="10">
+        <v>6</v>
+      </c>
+      <c r="H19" s="10">
+        <v>2</v>
+      </c>
+      <c r="I19" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="J19" s="61" t="s">
+        <v>100</v>
+      </c>
+      <c r="K19" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="L19" s="12" t="s">
+        <v>75</v>
+      </c>
+      <c r="M19" s="13">
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("ArrayFormula(mod(COUNTUNIQUE($C$3:C19),2))"),1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" ht="65.25" customHeight="1">
+      <c r="A20" s="32">
+        <v>1</v>
+      </c>
+      <c r="B20" s="14">
+        <v>2</v>
+      </c>
+      <c r="C20" s="28" t="s">
+        <v>94</v>
+      </c>
+      <c r="D20" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E20" s="37" t="s">
+        <v>59</v>
+      </c>
+      <c r="F20" s="15">
+        <v>3</v>
+      </c>
+      <c r="G20" s="15">
+        <v>6</v>
+      </c>
+      <c r="H20" s="15">
+        <v>3</v>
+      </c>
+      <c r="I20" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="L15" s="14" t="s">
-        <v>64</v>
-      </c>
-      <c r="M15" s="28">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("ArrayFormula(mod(COUNTUNIQUE($C$3:C15),2))"),1)</f>
+      <c r="J20" s="61" t="s">
+        <v>100</v>
+      </c>
+      <c r="K20" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="L20" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="M20" s="18">
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("ArrayFormula(mod(COUNTUNIQUE($C$3:C20),2))"),1)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="25.5">
-      <c r="A16" s="34" t="s">
+    <row r="21" spans="1:13" ht="64.5" customHeight="1">
+      <c r="A21" s="32">
+        <v>1</v>
+      </c>
+      <c r="B21" s="29">
+        <v>2</v>
+      </c>
+      <c r="C21" s="28" t="s">
         <v>94</v>
       </c>
-      <c r="B16" s="11">
-        <v>2</v>
-      </c>
-      <c r="C16" s="30" t="s">
-        <v>96</v>
-      </c>
-      <c r="D16" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="E16" s="39" t="s">
-        <v>60</v>
-      </c>
-      <c r="F16" s="12">
-        <v>2</v>
-      </c>
-      <c r="G16" s="12">
-        <v>5</v>
-      </c>
-      <c r="H16" s="12">
-        <v>2</v>
-      </c>
-      <c r="I16" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="J16" s="13"/>
-      <c r="K16" s="14" t="s">
-        <v>65</v>
-      </c>
-      <c r="L16" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="M16" s="15">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("ArrayFormula(mod(COUNTUNIQUE($C$3:C16),2))"),1)</f>
+      <c r="D21" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="E21" s="36" t="s">
+        <v>79</v>
+      </c>
+      <c r="F21" s="20">
+        <v>1</v>
+      </c>
+      <c r="G21" s="20">
+        <v>7</v>
+      </c>
+      <c r="H21" s="20">
+        <v>1</v>
+      </c>
+      <c r="I21" s="21" t="s">
+        <v>85</v>
+      </c>
+      <c r="J21" s="52" t="s">
+        <v>101</v>
+      </c>
+      <c r="K21" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="L21" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="M21" s="26">
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("ArrayFormula(mod(COUNTUNIQUE($C$3:C27),2))"),1)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="25.5">
-      <c r="A17" s="34" t="s">
+    <row r="22" spans="1:13" ht="64.5" customHeight="1">
+      <c r="A22" s="32">
+        <v>1</v>
+      </c>
+      <c r="B22" s="30">
+        <v>2</v>
+      </c>
+      <c r="C22" s="28" t="s">
         <v>94</v>
       </c>
-      <c r="B17" s="16">
-        <v>2</v>
-      </c>
-      <c r="C17" s="30" t="s">
-        <v>96</v>
-      </c>
-      <c r="D17" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="E17" s="41" t="s">
-        <v>60</v>
-      </c>
-      <c r="F17" s="17">
+      <c r="D22" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E22" s="35" t="s">
+        <v>79</v>
+      </c>
+      <c r="F22" s="10">
+        <v>2</v>
+      </c>
+      <c r="G22" s="10">
+        <v>7</v>
+      </c>
+      <c r="H22" s="10">
+        <v>2</v>
+      </c>
+      <c r="I22" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="J22" s="52" t="s">
+        <v>101</v>
+      </c>
+      <c r="K22" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="L22" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="M22" s="13">
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("ArrayFormula(mod(COUNTUNIQUE($C$3:C28),2))"),1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" ht="64.5" customHeight="1">
+      <c r="A23" s="32">
+        <v>1</v>
+      </c>
+      <c r="B23" s="30">
+        <v>2</v>
+      </c>
+      <c r="C23" s="28" t="s">
+        <v>94</v>
+      </c>
+      <c r="D23" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E23" s="35" t="s">
+        <v>79</v>
+      </c>
+      <c r="F23" s="10">
         <v>3</v>
       </c>
-      <c r="G17" s="17">
-        <v>5</v>
-      </c>
-      <c r="H17" s="17">
+      <c r="G23" s="10">
+        <v>7</v>
+      </c>
+      <c r="H23" s="10">
         <v>3</v>
       </c>
-      <c r="I17" s="18" t="s">
-        <v>63</v>
-      </c>
-      <c r="J17" s="18"/>
-      <c r="K17" s="19" t="s">
-        <v>67</v>
-      </c>
-      <c r="L17" s="19" t="s">
-        <v>68</v>
-      </c>
-      <c r="M17" s="15">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("ArrayFormula(mod(COUNTUNIQUE($C$3:C17),2))"),1)</f>
+      <c r="I23" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="J23" s="52" t="s">
+        <v>101</v>
+      </c>
+      <c r="K23" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="L23" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="M23" s="13">
+        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("ArrayFormula(mod(COUNTUNIQUE($C$3:C29),2))"),1)</f>
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="53.25" customHeight="1">
-      <c r="A18" s="36" t="s">
+    <row r="24" spans="1:13" ht="64.5" customHeight="1">
+      <c r="A24" s="32">
+        <v>1</v>
+      </c>
+      <c r="B24" s="9">
+        <v>2</v>
+      </c>
+      <c r="C24" s="28" t="s">
         <v>94</v>
       </c>
-      <c r="B18" s="11">
-        <v>2</v>
-      </c>
-      <c r="C18" s="30" t="s">
-        <v>96</v>
-      </c>
-      <c r="D18" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="E18" s="39" t="s">
-        <v>60</v>
-      </c>
-      <c r="F18" s="12">
-        <v>1</v>
-      </c>
-      <c r="G18" s="12">
-        <v>6</v>
-      </c>
-      <c r="H18" s="12">
-        <v>1</v>
-      </c>
-      <c r="I18" s="13" t="s">
-        <v>69</v>
-      </c>
-      <c r="J18" s="13"/>
-      <c r="K18" s="14" t="s">
-        <v>74</v>
-      </c>
-      <c r="L18" s="14" t="s">
-        <v>75</v>
-      </c>
-      <c r="M18" s="15">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("ArrayFormula(mod(COUNTUNIQUE($C$3:C18),2))"),1)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" ht="32.25" customHeight="1">
-      <c r="A19" s="36" t="s">
-        <v>94</v>
-      </c>
-      <c r="B19" s="11">
-        <v>2</v>
-      </c>
-      <c r="C19" s="30" t="s">
-        <v>96</v>
-      </c>
-      <c r="D19" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="E19" s="39" t="s">
-        <v>60</v>
-      </c>
-      <c r="F19" s="12">
-        <v>2</v>
-      </c>
-      <c r="G19" s="12">
-        <v>6</v>
-      </c>
-      <c r="H19" s="12">
-        <v>2</v>
-      </c>
-      <c r="I19" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="J19" s="13"/>
-      <c r="K19" s="14" t="s">
-        <v>73</v>
-      </c>
-      <c r="L19" s="14" t="s">
-        <v>76</v>
-      </c>
-      <c r="M19" s="15">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("ArrayFormula(mod(COUNTUNIQUE($C$3:C19),2))"),1)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" ht="60" customHeight="1">
-      <c r="A20" s="36" t="s">
-        <v>94</v>
-      </c>
-      <c r="B20" s="16">
-        <v>2</v>
-      </c>
-      <c r="C20" s="30" t="s">
-        <v>96</v>
-      </c>
-      <c r="D20" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="E20" s="41" t="s">
-        <v>60</v>
-      </c>
-      <c r="F20" s="17">
-        <v>3</v>
-      </c>
-      <c r="G20" s="17">
-        <v>6</v>
-      </c>
-      <c r="H20" s="17">
-        <v>3</v>
-      </c>
-      <c r="I20" s="18" t="s">
-        <v>72</v>
-      </c>
-      <c r="J20" s="18"/>
-      <c r="K20" s="19" t="s">
-        <v>77</v>
-      </c>
-      <c r="L20" s="19" t="s">
+      <c r="D24" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E24" s="35" t="s">
+        <v>79</v>
+      </c>
+      <c r="F24" s="10">
+        <v>1</v>
+      </c>
+      <c r="G24" s="10">
+        <v>8</v>
+      </c>
+      <c r="H24" s="10">
+        <v>1</v>
+      </c>
+      <c r="I24" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="M20" s="20">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("ArrayFormula(mod(COUNTUNIQUE($C$3:C20),2))"),1)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" ht="38.25">
-      <c r="A21" s="34" t="s">
-        <v>94</v>
-      </c>
-      <c r="B21" s="31">
-        <v>2</v>
-      </c>
-      <c r="C21" s="30" t="s">
-        <v>96</v>
-      </c>
-      <c r="D21" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="E21" s="40" t="s">
-        <v>80</v>
-      </c>
-      <c r="F21" s="22">
-        <v>1</v>
-      </c>
-      <c r="G21" s="22">
-        <v>7</v>
-      </c>
-      <c r="H21" s="22">
-        <v>1</v>
-      </c>
-      <c r="I21" s="23" t="s">
-        <v>86</v>
-      </c>
-      <c r="J21" s="23"/>
-      <c r="K21" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="L21" s="24" t="s">
-        <v>15</v>
-      </c>
-      <c r="M21" s="28">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("ArrayFormula(mod(COUNTUNIQUE($C$3:C27),2))"),1)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" ht="51">
-      <c r="A22" s="34" t="s">
-        <v>94</v>
-      </c>
-      <c r="B22" s="32">
-        <v>2</v>
-      </c>
-      <c r="C22" s="30" t="s">
-        <v>96</v>
-      </c>
-      <c r="D22" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="E22" s="39" t="s">
-        <v>80</v>
-      </c>
-      <c r="F22" s="12">
-        <v>2</v>
-      </c>
-      <c r="G22" s="12">
-        <v>7</v>
-      </c>
-      <c r="H22" s="12">
-        <v>2</v>
-      </c>
-      <c r="I22" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="J22" s="13"/>
-      <c r="K22" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="L22" s="14" t="s">
-        <v>93</v>
-      </c>
-      <c r="M22" s="15">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("ArrayFormula(mod(COUNTUNIQUE($C$3:C28),2))"),1)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" ht="63.75">
-      <c r="A23" s="34" t="s">
-        <v>94</v>
-      </c>
-      <c r="B23" s="32">
-        <v>2</v>
-      </c>
-      <c r="C23" s="30" t="s">
-        <v>96</v>
-      </c>
-      <c r="D23" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="E23" s="39" t="s">
-        <v>80</v>
-      </c>
-      <c r="F23" s="12">
-        <v>3</v>
-      </c>
-      <c r="G23" s="12">
-        <v>7</v>
-      </c>
-      <c r="H23" s="12">
-        <v>3</v>
-      </c>
-      <c r="I23" s="13" t="s">
+      <c r="J24" s="52" t="s">
+        <v>101</v>
+      </c>
+      <c r="K24" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="J23" s="13"/>
-      <c r="K23" s="14" t="s">
-        <v>17</v>
-      </c>
-      <c r="L23" s="14" t="s">
-        <v>92</v>
-      </c>
-      <c r="M23" s="15">
-        <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("ArrayFormula(mod(COUNTUNIQUE($C$3:C29),2))"),1)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" ht="38.25">
-      <c r="A24" s="36" t="s">
-        <v>94</v>
-      </c>
-      <c r="B24" s="11">
-        <v>2</v>
-      </c>
-      <c r="C24" s="30" t="s">
-        <v>96</v>
-      </c>
-      <c r="D24" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="E24" s="39" t="s">
-        <v>80</v>
-      </c>
-      <c r="F24" s="12">
-        <v>1</v>
-      </c>
-      <c r="G24" s="12">
-        <v>8</v>
-      </c>
-      <c r="H24" s="12">
-        <v>1</v>
-      </c>
-      <c r="I24" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="J24" s="13"/>
-      <c r="K24" s="14" t="s">
-        <v>89</v>
-      </c>
-      <c r="L24" s="14" t="s">
-        <v>83</v>
-      </c>
-      <c r="M24" s="26">
+      <c r="L24" s="12" t="s">
+        <v>82</v>
+      </c>
+      <c r="M24" s="24">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("ArrayFormula(mod(COUNTUNIQUE($C$3:C36),2))"),0)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:13" ht="38.25">
-      <c r="A25" s="36" t="s">
+    <row r="25" spans="1:13" ht="64.5" customHeight="1">
+      <c r="A25" s="32">
+        <v>1</v>
+      </c>
+      <c r="B25" s="9">
+        <v>2</v>
+      </c>
+      <c r="C25" s="28" t="s">
         <v>94</v>
       </c>
-      <c r="B25" s="11">
-        <v>2</v>
-      </c>
-      <c r="C25" s="30" t="s">
-        <v>96</v>
-      </c>
-      <c r="D25" s="12" t="s">
+      <c r="D25" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="E25" s="39" t="s">
+      <c r="E25" s="35" t="s">
+        <v>79</v>
+      </c>
+      <c r="F25" s="10">
+        <v>2</v>
+      </c>
+      <c r="G25" s="10">
+        <v>8</v>
+      </c>
+      <c r="H25" s="10">
+        <v>2</v>
+      </c>
+      <c r="I25" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="F25" s="12">
-        <v>2</v>
-      </c>
-      <c r="G25" s="12">
-        <v>8</v>
-      </c>
-      <c r="H25" s="12">
-        <v>2</v>
-      </c>
-      <c r="I25" s="13" t="s">
-        <v>81</v>
-      </c>
-      <c r="J25" s="13"/>
-      <c r="K25" s="14" t="s">
-        <v>90</v>
-      </c>
-      <c r="L25" s="14" t="s">
-        <v>84</v>
-      </c>
-      <c r="M25" s="26">
+      <c r="J25" s="52" t="s">
+        <v>101</v>
+      </c>
+      <c r="K25" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="L25" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="M25" s="24">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("ArrayFormula(mod(COUNTUNIQUE($C$3:C37),2))"),0)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:13" ht="51">
-      <c r="A26" s="36" t="s">
+    <row r="26" spans="1:13" ht="64.5" customHeight="1">
+      <c r="A26" s="32">
+        <v>1</v>
+      </c>
+      <c r="B26" s="14">
+        <v>2</v>
+      </c>
+      <c r="C26" s="28" t="s">
         <v>94</v>
       </c>
-      <c r="B26" s="16">
-        <v>2</v>
-      </c>
-      <c r="C26" s="30" t="s">
-        <v>96</v>
-      </c>
-      <c r="D26" s="17" t="s">
+      <c r="D26" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="E26" s="41" t="s">
-        <v>80</v>
-      </c>
-      <c r="F26" s="17">
+      <c r="E26" s="37" t="s">
+        <v>79</v>
+      </c>
+      <c r="F26" s="15">
         <v>3</v>
       </c>
-      <c r="G26" s="17">
+      <c r="G26" s="15">
         <v>8</v>
       </c>
-      <c r="H26" s="17">
+      <c r="H26" s="15">
         <v>3</v>
       </c>
-      <c r="I26" s="18" t="s">
-        <v>82</v>
-      </c>
-      <c r="J26" s="18"/>
-      <c r="K26" s="19" t="s">
-        <v>91</v>
-      </c>
-      <c r="L26" s="19" t="s">
-        <v>85</v>
-      </c>
-      <c r="M26" s="27">
+      <c r="I26" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="J26" s="52" t="s">
+        <v>101</v>
+      </c>
+      <c r="K26" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="L26" s="17" t="s">
+        <v>84</v>
+      </c>
+      <c r="M26" s="25">
         <f ca="1">IFERROR(__xludf.DUMMYFUNCTION("ArrayFormula(mod(COUNTUNIQUE($C$3:C38),2))"),0)</f>
         <v>0</v>
       </c>
@@ -2373,157 +2495,174 @@
       </autoFilter>
     </customSheetView>
   </customSheetViews>
-  <conditionalFormatting sqref="B3:L5 M3:M26 B24:L26 C4:C26">
-    <cfRule type="expression" dxfId="35" priority="29">
+  <conditionalFormatting sqref="M3:M26 B24:L26 C4:C26 B3:L5">
+    <cfRule type="expression" dxfId="31" priority="31">
       <formula>$M3=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B3:L5 M3:M26 B24:L26 C4:C26">
-    <cfRule type="expression" dxfId="34" priority="31">
+  <conditionalFormatting sqref="M3:M26 B24:L26 C4:C26 B3:L5">
+    <cfRule type="expression" dxfId="30" priority="33">
       <formula>$M3=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B21:L23">
-    <cfRule type="expression" dxfId="33" priority="52">
+  <conditionalFormatting sqref="B21:L23 J22:J26">
+    <cfRule type="expression" dxfId="29" priority="54">
       <formula>#REF!=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B21:L23">
-    <cfRule type="expression" dxfId="32" priority="53">
+  <conditionalFormatting sqref="B21:L23 J22:J26">
+    <cfRule type="expression" dxfId="28" priority="55">
       <formula>#REF!=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B15:L17">
-    <cfRule type="expression" dxfId="31" priority="62">
+  <conditionalFormatting sqref="B15:L17 J18:J20">
+    <cfRule type="expression" dxfId="27" priority="64">
       <formula>$M6=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B15:L17">
-    <cfRule type="expression" dxfId="30" priority="64">
+  <conditionalFormatting sqref="B15:L17 J18:J20">
+    <cfRule type="expression" dxfId="26" priority="66">
       <formula>$M6=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B6:L8 C12:C14 C18:C20 C24:C26">
-    <cfRule type="expression" dxfId="29" priority="66">
+  <conditionalFormatting sqref="C12:C14 C18:C20 C24:C26 B6:L8">
+    <cfRule type="expression" dxfId="25" priority="68">
       <formula>$M9=1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B6:L8 C12:C14 C18:C20 C24:C26">
-    <cfRule type="expression" dxfId="28" priority="68">
+  <conditionalFormatting sqref="C12:C14 C18:C20 C24:C26 B6:L8">
+    <cfRule type="expression" dxfId="24" priority="70">
       <formula>$M9=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18:L20">
-    <cfRule type="expression" dxfId="27" priority="70">
+    <cfRule type="expression" dxfId="23" priority="72">
       <formula>$M12=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18:L20">
-    <cfRule type="expression" dxfId="26" priority="72">
+    <cfRule type="expression" dxfId="22" priority="74">
       <formula>$M12=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9:L14">
-    <cfRule type="expression" dxfId="25" priority="74">
+    <cfRule type="expression" dxfId="21" priority="76">
       <formula>$M15=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B9:L14">
-    <cfRule type="expression" dxfId="24" priority="76">
+    <cfRule type="expression" dxfId="20" priority="78">
       <formula>$M15=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I9:I14">
-    <cfRule type="expression" dxfId="23" priority="18">
+    <cfRule type="expression" dxfId="19" priority="20">
       <formula>$Y9=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I9:I14">
-    <cfRule type="expression" dxfId="22" priority="17">
+    <cfRule type="expression" dxfId="18" priority="19">
       <formula>$Y9=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E12:E14">
-    <cfRule type="expression" dxfId="21" priority="16">
+    <cfRule type="expression" dxfId="17" priority="18">
       <formula>$Y12=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E12:E14">
-    <cfRule type="expression" dxfId="20" priority="15">
+    <cfRule type="expression" dxfId="16" priority="17">
       <formula>$Y12=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I12:I14">
-    <cfRule type="expression" dxfId="19" priority="14">
+    <cfRule type="expression" dxfId="15" priority="16">
       <formula>$Y12=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I12:I14">
-    <cfRule type="expression" dxfId="18" priority="13">
+    <cfRule type="expression" dxfId="14" priority="15">
       <formula>$Y12=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I12:I14">
-    <cfRule type="expression" dxfId="17" priority="12">
+    <cfRule type="expression" dxfId="13" priority="14">
       <formula>$Y12=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I12:I14">
-    <cfRule type="expression" dxfId="16" priority="11">
+    <cfRule type="expression" dxfId="12" priority="13">
       <formula>$Y12=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K12:K14">
-    <cfRule type="expression" dxfId="15" priority="10">
+    <cfRule type="expression" dxfId="11" priority="12">
       <formula>$Y12=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K12:K14">
-    <cfRule type="expression" dxfId="14" priority="9">
+    <cfRule type="expression" dxfId="10" priority="11">
       <formula>$Y12=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L12:L14">
-    <cfRule type="expression" dxfId="13" priority="8">
+    <cfRule type="expression" dxfId="9" priority="10">
       <formula>$Y12=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L12:L14">
-    <cfRule type="expression" dxfId="12" priority="7">
+    <cfRule type="expression" dxfId="8" priority="9">
       <formula>$Y12=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I24:I26">
-    <cfRule type="expression" dxfId="11" priority="6">
+    <cfRule type="expression" dxfId="7" priority="8">
       <formula>$Y24=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I24:I26">
-    <cfRule type="expression" dxfId="10" priority="5">
+    <cfRule type="expression" dxfId="6" priority="7">
       <formula>$Y24=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K24:K26">
-    <cfRule type="expression" dxfId="9" priority="4">
+    <cfRule type="expression" dxfId="5" priority="6">
       <formula>$Y24=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K24:K26">
-    <cfRule type="expression" dxfId="8" priority="3">
+    <cfRule type="expression" dxfId="4" priority="5">
       <formula>$Y24=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L25:L26">
-    <cfRule type="expression" dxfId="7" priority="2">
+    <cfRule type="expression" dxfId="3" priority="4">
       <formula>$Y25=1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L25:L26">
-    <cfRule type="expression" dxfId="6" priority="1">
+    <cfRule type="expression" dxfId="2" priority="3">
       <formula>$Y25=0</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="J3:J5">
+    <cfRule type="expression" dxfId="1" priority="2">
+      <formula>$M3=1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J3:J5">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>$M3=0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="J12" r:id="rId1" location="pictogram"/>
+    <hyperlink ref="J13:J14" r:id="rId2" location="pictogram" display="https://www.j2e.com/jit5#pictogram"/>
+    <hyperlink ref="J15" r:id="rId3"/>
+    <hyperlink ref="J16:J17" r:id="rId4" display="https://musiclab.chromeexperiments.com/"/>
+    <hyperlink ref="J18:J20" r:id="rId5" display="https://musiclab.chromeexperiments.com/"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>